<commit_message>
Add readme + code review
</commit_message>
<xml_diff>
--- a/Sprint 2 Deliverables/Sprint 2 Tasks.xlsx
+++ b/Sprint 2 Deliverables/Sprint 2 Tasks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tingy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukes\OneDrive\Desktop\Repositories\Sprint1\Sprint 2 Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43851F1-45F0-48AB-8051-29A301FD6562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A268E5B4-C6E1-4A98-A058-BEE8A1ABE25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="start-from-scratch" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -118,9 +118,6 @@
     <t>Tile Refactoring, Player Refactoring, Projectile Refactoring, Enemy Refactoring</t>
   </si>
   <si>
-    <t>Working on it</t>
-  </si>
-  <si>
     <t>Tile Refactoring</t>
   </si>
   <si>
@@ -172,9 +169,6 @@
     <t>Sprint 2 Tasks</t>
   </si>
   <si>
-    <t>Group Name: Systems 1 is My Favorite Class</t>
-  </si>
-  <si>
     <t>Task Names</t>
   </si>
   <si>
@@ -191,6 +185,9 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>Group Name: Team 6</t>
   </si>
 </sst>
 </file>
@@ -198,9 +195,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -253,14 +250,8 @@
       <name val="Arial"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="1"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,16 +285,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFDAB3D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -326,26 +312,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color rgb="FFE99729"/>
-      </left>
-      <right style="thick">
-        <color rgb="FFE99729"/>
-      </right>
-      <top style="thick">
-        <color rgb="FFE99729"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFE99729"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -365,7 +336,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -377,13 +348,10 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -748,7 +716,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -762,20 +730,20 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>2</v>
@@ -784,7 +752,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -795,7 +763,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>7</v>
@@ -897,7 +865,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>7</v>
@@ -965,7 +933,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>7</v>
@@ -1033,7 +1001,7 @@
         <v>23</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>7</v>
@@ -1101,7 +1069,7 @@
         <v>27</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>7</v>
@@ -1169,10 +1137,10 @@
         <v>31</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>32</v>
+        <v>54</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="E26" s="7">
         <v>44613</v>
@@ -1200,10 +1168,10 @@
         <v>9</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>7</v>
@@ -1217,10 +1185,10 @@
         <v>9</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>7</v>
@@ -1234,10 +1202,10 @@
         <v>9</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>7</v>
@@ -1251,13 +1219,13 @@
         <v>9</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>32</v>
+        <v>41</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="E31" s="7">
         <v>44613</v>
@@ -1265,16 +1233,16 @@
     </row>
     <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="C32" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="11" t="s">
-        <v>32</v>
+      <c r="D32" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="E32" s="7">
         <v>44613</v>
@@ -1305,10 +1273,10 @@
         <v>22</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>32</v>
+        <v>41</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="E34" s="7">
         <v>44613</v>
@@ -1322,10 +1290,10 @@
         <v>18</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>32</v>
+        <v>42</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="E35" s="7">
         <v>44613</v>
@@ -1339,10 +1307,10 @@
         <v>5</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="E36" s="7">
         <v>44613</v>
@@ -1356,10 +1324,10 @@
         <v>26</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>32</v>
+        <v>40</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="E37" s="7">
         <v>44613</v>
@@ -1370,13 +1338,13 @@
         <v>9</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="E38" s="7">
         <v>44613</v>
@@ -1384,16 +1352,16 @@
     </row>
     <row r="39" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="8" t="s">
-        <v>45</v>
-      </c>
       <c r="C39" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="11" t="s">
-        <v>32</v>
+      <c r="D39" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>9</v>
@@ -1421,13 +1389,13 @@
         <v>9</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>32</v>
+        <v>40</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="E41" s="7">
         <v>44613</v>
@@ -1438,13 +1406,13 @@
         <v>9</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>32</v>
+        <v>40</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="E42" s="7">
         <v>44613</v>
@@ -1455,13 +1423,13 @@
         <v>9</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="E43" s="7">
         <v>44613</v>
@@ -1480,8 +1448,8 @@
       <c r="D44" t="s">
         <v>9</v>
       </c>
-      <c r="E44" s="13" t="s">
-        <v>53</v>
+      <c r="E44" s="12" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>